<commit_message>
aktualizace tabs a FliudSim picture added
</commit_message>
<xml_diff>
--- a/Tabs.xlsx
+++ b/Tabs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Denisa\Desktop\ŘPA\Semestrálka\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PSorf\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E26ABCC-4696-41BE-AC8C-32B4B695ABA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A9B4A0-5930-4949-AED9-C9B8C55BCFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{CE0766FF-EFC9-4C7A-97E5-8CA936E30FB8}"/>
+    <workbookView xWindow="-19320" yWindow="660" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{CE0766FF-EFC9-4C7A-97E5-8CA936E30FB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Stavová diagram" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="132">
   <si>
     <t>Stav</t>
   </si>
@@ -366,9 +366,6 @@
     <t>Q0.0</t>
   </si>
   <si>
-    <t>Q0.1</t>
-  </si>
-  <si>
     <t>Q0.2</t>
   </si>
   <si>
@@ -390,21 +387,12 @@
     <t>Spustění</t>
   </si>
   <si>
-    <t>YA0</t>
-  </si>
-  <si>
     <t>YA1</t>
   </si>
   <si>
-    <t>YB0</t>
-  </si>
-  <si>
     <t>YB1</t>
   </si>
   <si>
-    <t>YC0</t>
-  </si>
-  <si>
     <t>YC1</t>
   </si>
   <si>
@@ -442,6 +430,12 @@
   </si>
   <si>
     <t>MANUAL = 1</t>
+  </si>
+  <si>
+    <t>Q0.3</t>
+  </si>
+  <si>
+    <t>YA2</t>
   </si>
 </sst>
 </file>
@@ -648,8 +642,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3A912FEE-3924-486F-95E2-96CD619A8A1D}" name="Tabulka48" displayName="Tabulka48" ref="A2:C15" totalsRowShown="0">
-  <autoFilter ref="A2:C15" xr:uid="{3A912FEE-3924-486F-95E2-96CD619A8A1D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3A912FEE-3924-486F-95E2-96CD619A8A1D}" name="Tabulka48" displayName="Tabulka48" ref="A2:C13" totalsRowShown="0">
+  <autoFilter ref="A2:C13" xr:uid="{3A912FEE-3924-486F-95E2-96CD619A8A1D}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{46C420DF-769B-49E1-9829-DD2E7BFB06BD}" name="Název"/>
     <tableColumn id="2" xr3:uid="{23682907-CA77-4D73-8D1A-351227EB9976}" name="Adresa"/>
@@ -660,8 +654,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{CE587967-EC0E-47AC-861F-FAC83961D81A}" name="Tabulka59" displayName="Tabulka59" ref="A18:C24" totalsRowShown="0">
-  <autoFilter ref="A18:C24" xr:uid="{CE587967-EC0E-47AC-861F-FAC83961D81A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{CE587967-EC0E-47AC-861F-FAC83961D81A}" name="Tabulka59" displayName="Tabulka59" ref="A16:C22" totalsRowShown="0">
+  <autoFilter ref="A16:C22" xr:uid="{CE587967-EC0E-47AC-861F-FAC83961D81A}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{69096A12-63BC-4C8F-A4EF-CF983439AC97}" name="Název"/>
     <tableColumn id="2" xr3:uid="{3331E8B8-A9F4-4088-BE00-6FECE382BC6A}" name="Adresa"/>
@@ -1274,7 +1268,7 @@
         <v>88</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1317,13 +1311,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" s="3">
         <v>10001</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1338,14 +1332,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{568BA240-2221-49D0-A268-F018AA0252FC}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.21875" customWidth="1"/>
-    <col min="3" max="3" width="30.88671875" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -1498,13 +1492,13 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" t="s">
         <v>112</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>113</v>
-      </c>
-      <c r="C15" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -1550,7 +1544,7 @@
         <v>103</v>
       </c>
       <c r="B21" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="C21" t="s">
         <v>106</v>
@@ -1568,10 +1562,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7E5F274-3DF1-4054-B3A1-6B57D7787E2E}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1601,7 +1595,7 @@
         <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1661,160 +1655,138 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B9" t="s">
         <v>81</v>
       </c>
       <c r="C9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s">
         <v>82</v>
       </c>
       <c r="C10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
         <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
       <c r="C13" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>121</v>
-      </c>
-      <c r="B14" t="s">
-        <v>86</v>
-      </c>
-      <c r="C14" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>112</v>
-      </c>
-      <c r="B15" t="s">
-        <v>113</v>
-      </c>
-      <c r="C15" t="s">
-        <v>114</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>69</v>
+      </c>
+      <c r="B17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C22" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" t="s">
-        <v>85</v>
-      </c>
-      <c r="C23" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>74</v>
-      </c>
-      <c r="B24" t="s">
-        <v>86</v>
-      </c>
-      <c r="C24" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1843,34 +1815,34 @@
   <sheetData>
     <row r="2" spans="10:11" x14ac:dyDescent="0.3">
       <c r="J2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="K2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="10:11" x14ac:dyDescent="0.3">
       <c r="J3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="K3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="10:11" x14ac:dyDescent="0.3">
       <c r="J4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="K4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="10:11" x14ac:dyDescent="0.3">
       <c r="J5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="K5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>